<commit_message>
Worked on some graphs
</commit_message>
<xml_diff>
--- a/paper/raw_data/revised/old_results/exp04_COMPARISON_OC.xlsx
+++ b/paper/raw_data/revised/old_results/exp04_COMPARISON_OC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Desktop\MemPod\paper\raw_data\revised\old_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Documents\UCSD\MigrationResearch\MemPod\paper\raw_data\revised\old_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -202,13 +202,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1890,7 +1890,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$Q$2</c15:sqref>
@@ -1919,7 +1919,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$K$3:$K$32</c15:sqref>
@@ -2023,7 +2023,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$Q$3:$Q$32</c15:sqref>
@@ -2126,7 +2126,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A30C-4D75-9F32-A7C62C551628}"/>
                   </c:ext>
@@ -2482,12 +2482,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2532,12 +2529,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2545,14 +2539,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="900" b="1"/>
-                  <a:t>AMMAT</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AMMAT / AMMAT (DDR4-2400)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="900" b="1" baseline="0"/>
-                  <a:t> / AMMAT (DDR4-2400)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="900" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2569,12 +2558,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2601,12 +2587,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2652,7 +2635,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr b="1">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3760,15 +3747,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>157164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4093,14 +4080,14 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="10" max="10" width="2.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="10" max="10" width="2.1328125" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
@@ -4114,66 +4101,66 @@
       <c r="L1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -4200,7 +4187,7 @@
       <c r="I3">
         <v>12.37</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L3">
@@ -4236,8 +4223,8 @@
         <v>0.37047020065887987</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -4264,7 +4251,7 @@
       <c r="I4">
         <v>28.86</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="L4">
@@ -4300,8 +4287,8 @@
         <v>0.58385595792029132</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -4328,7 +4315,7 @@
       <c r="I5">
         <v>55.82</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L5">
@@ -4364,8 +4351,8 @@
         <v>0.63252124645892349</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6">
@@ -4392,7 +4379,7 @@
       <c r="I6">
         <v>35.549999999999997</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L6">
@@ -4428,8 +4415,8 @@
         <v>0.36353410369158395</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7">
@@ -4456,7 +4443,7 @@
       <c r="I7">
         <v>57.67</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L7">
@@ -4492,8 +4479,8 @@
         <v>0.69750846637639086</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8">
@@ -4521,7 +4508,7 @@
         <f>B8*2/3</f>
         <v>16.533333333333335</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L8">
@@ -4557,8 +4544,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9">
@@ -4585,7 +4572,7 @@
       <c r="I9">
         <v>22.22</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L9">
@@ -4621,8 +4608,8 @@
         <v>0.40928347762018785</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10">
@@ -4649,7 +4636,7 @@
       <c r="I10">
         <v>7.49</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L10">
@@ -4685,8 +4672,8 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11">
@@ -4713,7 +4700,7 @@
       <c r="I11">
         <v>28.29</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="L11">
@@ -4749,8 +4736,8 @@
         <v>0.46059915337023766</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12">
@@ -4777,7 +4764,7 @@
       <c r="I12">
         <v>11.01</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="L12">
@@ -4813,8 +4800,8 @@
         <v>0.32660931474339955</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13">
@@ -4841,7 +4828,7 @@
       <c r="I13">
         <v>13.68</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L13">
@@ -4877,8 +4864,8 @@
         <v>0.36142668428005281</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14">
@@ -4905,7 +4892,7 @@
       <c r="I14">
         <v>9.0299999999999994</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L14">
@@ -4941,8 +4928,8 @@
         <v>0.32587513533020568</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15">
@@ -4969,7 +4956,7 @@
       <c r="I15">
         <v>22.87</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L15">
@@ -5005,8 +4992,8 @@
         <v>0.43611746758199849</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B16">
@@ -5033,7 +5020,7 @@
       <c r="I16">
         <v>51.52</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L16">
@@ -5069,8 +5056,8 @@
         <v>0.60912745329865225</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17">
@@ -5097,7 +5084,7 @@
       <c r="I17">
         <v>28.69</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L17">
@@ -5133,8 +5120,8 @@
         <v>0.46940445026178013</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18">
@@ -5161,7 +5148,7 @@
       <c r="I18">
         <v>15.59</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L18">
@@ -5197,8 +5184,8 @@
         <v>0.36314931283484742</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19">
@@ -5225,7 +5212,7 @@
       <c r="I19">
         <v>10.55</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="L19">
@@ -5261,8 +5248,8 @@
         <v>0.31075110456553756</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20">
@@ -5289,7 +5276,7 @@
       <c r="I20">
         <v>19.809999999999999</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L20">
@@ -5325,8 +5312,8 @@
         <v>0.40428571428571425</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21">
@@ -5353,7 +5340,7 @@
       <c r="I21">
         <v>37.07</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L21">
@@ -5389,8 +5376,8 @@
         <v>0.45240419819380034</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22">
@@ -5417,7 +5404,7 @@
       <c r="I22">
         <v>19.170000000000002</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="L22">
@@ -5453,8 +5440,8 @@
         <v>0.40743889479277373</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23">
@@ -5481,7 +5468,7 @@
       <c r="I23">
         <v>12.69</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L23">
@@ -5517,8 +5504,8 @@
         <v>0.33115866388308973</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24">
@@ -5545,7 +5532,7 @@
       <c r="I24">
         <v>19.14</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="L24">
@@ -5581,8 +5568,8 @@
         <v>0.39693073413521363</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B25">
@@ -5609,7 +5596,7 @@
       <c r="I25">
         <v>23.72</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L25">
@@ -5645,8 +5632,8 @@
         <v>0.39818700688265901</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26">
@@ -5673,7 +5660,7 @@
       <c r="I26">
         <v>17.95</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L26">
@@ -5709,8 +5696,8 @@
         <v>0.36964579901153211</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B27">
@@ -5737,7 +5724,7 @@
       <c r="I27">
         <v>26.58</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L27">
@@ -5773,8 +5760,8 @@
         <v>0.46081830790568651</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B28">
@@ -5801,7 +5788,7 @@
       <c r="I28">
         <v>25</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L28">
@@ -5837,8 +5824,8 @@
         <v>0.43237634036665512</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B29">
@@ -5865,7 +5852,7 @@
       <c r="I29">
         <v>20.43</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L29">
@@ -5901,8 +5888,8 @@
         <v>0.41297756215888415</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B30">
@@ -5910,7 +5897,7 @@
         <v>54.96400000000002</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:S30" si="9">AVERAGE(C3:C17)</f>
+        <f t="shared" ref="C30:I30" si="9">AVERAGE(C3:C17)</f>
         <v>42.145333333333333</v>
       </c>
       <c r="D30">
@@ -5937,7 +5924,7 @@
         <f t="shared" si="9"/>
         <v>26.773555555555554</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L30">
@@ -5973,8 +5960,8 @@
         <v>0.48711075532267561</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B31">
@@ -5982,7 +5969,7 @@
         <v>51.209166666666668</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:S31" si="10">AVERAGE(C18:C29)</f>
+        <f t="shared" ref="C31:I31" si="10">AVERAGE(C18:C29)</f>
         <v>36.38750000000001</v>
       </c>
       <c r="D31">
@@ -6009,7 +5996,7 @@
         <f t="shared" si="10"/>
         <v>20.641666666666666</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L31">
@@ -6045,8 +6032,8 @@
         <v>0.40308538510357844</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B32">
@@ -6054,7 +6041,7 @@
         <v>53.295185185185183</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:S32" si="11">AVERAGE(C3:C29)</f>
+        <f t="shared" ref="C32:I32" si="11">AVERAGE(C3:C29)</f>
         <v>39.586296296296297</v>
       </c>
       <c r="D32">
@@ -6081,7 +6068,7 @@
         <f t="shared" si="11"/>
         <v>24.048271604938275</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="L32">
@@ -6117,33 +6104,33 @@
         <v>0.451227845843439</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.45">
       <c r="D34">
         <f>D32/C32</f>
         <v>0.88495831890946175</v>
@@ -6161,31 +6148,31 @@
         <v>0.60748980972964217</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="L37" s="4" t="s">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="L37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="4" t="s">
+      <c r="N37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O37" s="4" t="s">
+      <c r="O37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P37" s="4" t="s">
+      <c r="P37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q37" s="4" t="s">
+      <c r="Q37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K38" s="4" t="s">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="K38" s="2" t="s">
         <v>39</v>
       </c>
       <c r="L38">

</xml_diff>

<commit_message>
Fixed typos and minor modifications based on Nuwan's comments. Need to trip the paper by one column
</commit_message>
<xml_diff>
--- a/paper/raw_data/revised/old_results/exp04_COMPARISON_OC.xlsx
+++ b/paper/raw_data/revised/old_results/exp04_COMPARISON_OC.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Documents\UCSD\MigrationResearch\MemPod\paper\raw_data\revised\old_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprodrom\Desktop\MemPod\paper\raw_data\revised\old_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,10 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -158,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,7 +227,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -473,7 +470,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -702,7 +699,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -931,7 +928,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -1160,7 +1157,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -1389,7 +1386,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -1618,7 +1615,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-A30C-4D75-9F32-A7C62C551628}"/>
             </c:ext>
@@ -1634,9 +1631,9 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="370010536"/>
-        <c:axId val="370016440"/>
-        <c:extLst>
+        <c:axId val="379708608"/>
+        <c:axId val="379709000"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
               <c15:ser>
@@ -1644,7 +1641,7 @@
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$2</c15:sqref>
@@ -1673,7 +1670,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$K$3:$K$32</c15:sqref>
@@ -1777,7 +1774,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$3:$L$32</c15:sqref>
@@ -1880,7 +1877,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-A30C-4D75-9F32-A7C62C551628}"/>
                   </c:ext>
@@ -1893,7 +1890,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$Q$2</c15:sqref>
@@ -1922,7 +1919,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$K$3:$K$32</c15:sqref>
@@ -2026,7 +2023,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$Q$3:$Q$32</c15:sqref>
@@ -2129,7 +2126,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A30C-4D75-9F32-A7C62C551628}"/>
                   </c:ext>
@@ -2140,7 +2137,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="370010536"/>
+        <c:axId val="379708608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,7 +2180,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370016440"/>
+        <c:crossAx val="379709000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="370016440"/>
+        <c:axId val="379709000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -2243,7 +2240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="370010536"/>
+        <c:crossAx val="379708608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2257,6 +2254,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2324,7 +2322,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2429,7 +2427,7 @@
                   <c:v>0.65732433615711239</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57902527502310697</c:v>
+                  <c:v>0.57335455221443121</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.451227845843439</c:v>
@@ -2437,7 +2435,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8EB4-42F8-ACD7-B2CF1A834764}"/>
             </c:ext>
@@ -2453,11 +2451,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="360132736"/>
-        <c:axId val="360134704"/>
+        <c:axId val="379709392"/>
+        <c:axId val="379710960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="360132736"/>
+        <c:axId val="379709392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360134704"/>
+        <c:crossAx val="379710960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2505,7 +2503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="360134704"/>
+        <c:axId val="379710960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,6 +2546,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2602,7 +2601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360132736"/>
+        <c:crossAx val="379709392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3719,16 +3718,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9523</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333373</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3778,227 +3777,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="NUM_MEA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="42">
-          <cell r="B42">
-            <v>16</v>
-          </cell>
-          <cell r="K42">
-            <v>1</v>
-          </cell>
-          <cell r="S42">
-            <v>5.5293333333333345</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>32</v>
-          </cell>
-          <cell r="K43">
-            <v>0.97144305784988805</v>
-          </cell>
-          <cell r="S43">
-            <v>9.8260000000000005</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>64</v>
-          </cell>
-          <cell r="K44">
-            <v>0.94605910927201053</v>
-          </cell>
-          <cell r="S44">
-            <v>16.27333333333333</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>AVG HG</v>
-          </cell>
-          <cell r="B45">
-            <v>128</v>
-          </cell>
-          <cell r="K45">
-            <v>0.93789764642384021</v>
-          </cell>
-          <cell r="S45">
-            <v>24.355999999999995</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>256</v>
-          </cell>
-          <cell r="K46">
-            <v>0.93582048052861433</v>
-          </cell>
-          <cell r="S46">
-            <v>31.40333333333334</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>512</v>
-          </cell>
-          <cell r="K47">
-            <v>0.95070411017157086</v>
-          </cell>
-          <cell r="S47">
-            <v>39.788000000000004</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>16</v>
-          </cell>
-          <cell r="L49">
-            <v>1</v>
-          </cell>
-          <cell r="T49">
-            <v>7.3083333333333336</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>32</v>
-          </cell>
-          <cell r="L50">
-            <v>0.96679464326523112</v>
-          </cell>
-          <cell r="T50">
-            <v>13.094999999999999</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>64</v>
-          </cell>
-          <cell r="L51">
-            <v>0.94334750217103147</v>
-          </cell>
-          <cell r="T51">
-            <v>22.46083333333333</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>AVG MIX</v>
-          </cell>
-          <cell r="B52">
-            <v>128</v>
-          </cell>
-          <cell r="L52">
-            <v>0.93841126194067359</v>
-          </cell>
-          <cell r="T52">
-            <v>36.655833333333341</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>256</v>
-          </cell>
-          <cell r="L53">
-            <v>0.94357603181132599</v>
-          </cell>
-          <cell r="T53">
-            <v>52.180833333333339</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>512</v>
-          </cell>
-          <cell r="L54">
-            <v>0.9646921705745235</v>
-          </cell>
-          <cell r="T54">
-            <v>72.006666666666661</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>16</v>
-          </cell>
-          <cell r="M56">
-            <v>1</v>
-          </cell>
-          <cell r="U56">
-            <v>6.3200000000000012</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>32</v>
-          </cell>
-          <cell r="M57">
-            <v>0.96950399908483431</v>
-          </cell>
-          <cell r="U57">
-            <v>11.27888888888889</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58">
-            <v>64</v>
-          </cell>
-          <cell r="M58">
-            <v>0.94492797834107123</v>
-          </cell>
-          <cell r="U58">
-            <v>19.02333333333333</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>AVG ALL</v>
-          </cell>
-          <cell r="B59">
-            <v>128</v>
-          </cell>
-          <cell r="M59">
-            <v>0.93811189811151718</v>
-          </cell>
-          <cell r="U59">
-            <v>29.822592592592596</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>256</v>
-          </cell>
-          <cell r="M60">
-            <v>0.93905566306637855</v>
-          </cell>
-          <cell r="U60">
-            <v>40.637777777777771</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61">
-            <v>512</v>
-          </cell>
-          <cell r="M61">
-            <v>0.95653914717966837</v>
-          </cell>
-          <cell r="U61">
-            <v>54.107407407407393</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4300,18 +4078,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="10" max="10" width="2.1328125" customWidth="1"/>
-    <col min="11" max="11" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="10" max="10" width="2.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
@@ -4333,7 +4111,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4383,7 +4161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -4447,7 +4225,7 @@
         <v>0.37047020065887987</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -4511,7 +4289,7 @@
         <v>0.58385595792029132</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4575,7 +4353,7 @@
         <v>0.63252124645892349</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -4639,7 +4417,7 @@
         <v>0.36353410369158395</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -4703,7 +4481,7 @@
         <v>0.69750846637639086</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -4768,7 +4546,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4832,7 +4610,7 @@
         <v>0.40928347762018785</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -4896,7 +4674,7 @@
         <v>0.214</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -4960,7 +4738,7 @@
         <v>0.46059915337023766</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -5024,7 +4802,7 @@
         <v>0.32660931474339955</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -5088,7 +4866,7 @@
         <v>0.36142668428005281</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5152,7 +4930,7 @@
         <v>0.32587513533020568</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5216,7 +4994,7 @@
         <v>0.43611746758199849</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -5280,7 +5058,7 @@
         <v>0.60912745329865225</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -5344,7 +5122,7 @@
         <v>0.46940445026178013</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -5408,7 +5186,7 @@
         <v>0.36314931283484742</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -5472,7 +5250,7 @@
         <v>0.31075110456553756</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -5536,7 +5314,7 @@
         <v>0.40428571428571425</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -5600,7 +5378,7 @@
         <v>0.45240419819380034</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -5664,7 +5442,7 @@
         <v>0.40743889479277373</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -5728,7 +5506,7 @@
         <v>0.33115866388308973</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -5792,7 +5570,7 @@
         <v>0.39693073413521363</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -5856,7 +5634,7 @@
         <v>0.39818700688265901</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -5920,7 +5698,7 @@
         <v>0.36964579901153211</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -5984,7 +5762,7 @@
         <v>0.46081830790568651</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -6048,7 +5826,7 @@
         <v>0.43237634036665512</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -6112,7 +5890,7 @@
         <v>0.41297756215888415</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -6184,7 +5962,7 @@
         <v>0.48711075532267561</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -6256,7 +6034,7 @@
         <v>0.40308538510357844</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -6328,7 +6106,7 @@
         <v>0.451227845843439</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
@@ -6354,7 +6132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D34">
         <f>D32/C32</f>
         <v>0.88495831890946175</v>
@@ -6367,12 +6145,16 @@
         <f>F32/C32</f>
         <v>0.77954398735065455</v>
       </c>
+      <c r="G34">
+        <f>G32/C32</f>
+        <v>0.7719094711039175</v>
+      </c>
       <c r="I34">
         <f>I32/C32</f>
         <v>0.60748980972964217</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="L37" s="2" t="s">
         <v>0</v>
       </c>
@@ -6395,7 +6177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K38" s="2" t="s">
         <v>39</v>
       </c>
@@ -6415,7 +6197,7 @@
         <v>0.65732433615711239</v>
       </c>
       <c r="Q38">
-        <v>0.57902527502310697</v>
+        <v>0.57335455221443121</v>
       </c>
       <c r="R38">
         <v>0.451227845843439</v>

</xml_diff>